<commit_message>
lagt inn data i skjema
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,26 +468,26 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Berit Andresen</t>
+          <t>Lars Arne</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Festningsgata 2</t>
+          <t>dronningsgata 7</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>90832301</t>
+          <t>92807453</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10018093002</t>
+          <t>10118873035</t>
         </is>
       </c>
     </row>
@@ -496,27 +496,75 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Henning Berg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>festningsgata 12</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>90806450</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>08127995110</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Berit Andresen</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Festningsgata 2</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>90832301</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10018093002</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Lars Arne Holt</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Jeving veien 4</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>90492508</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>12108795110</t>
-        </is>
+      <c r="E5" t="n">
+        <v>90492508</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12108795110</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -729,9 +777,18 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -744,7 +801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -819,25 +876,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
@@ -845,20 +894,61 @@
           <t>Fjelltoppen barnehage</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2024-08-18</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>800000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>on</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Fjelltoppen barnehage</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>2020-09-18</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
+      <c r="M3" t="n">
+        <v>1500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
endret data på nettsiden
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,26 +468,26 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lars Arne</t>
+          <t>Berit Hansen</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>dronningsgata 7</t>
+          <t>Kongensgate 3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>92807453</t>
+          <t>91098791</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10118873035</t>
+          <t>09030072561</t>
         </is>
       </c>
     </row>
@@ -496,26 +496,26 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Henning Berg</t>
+          <t>Per Johansen</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>festningsgata 12</t>
+          <t>Vabråten 100</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>90806450</t>
+          <t>98726451</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>08127995110</t>
+          <t>10029085321</t>
         </is>
       </c>
     </row>
@@ -524,23 +524,23 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Berit Andresen</t>
+          <t>Lars Arne</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Festningsgata 2</t>
+          <t>dronningsgata 7</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>90832301</v>
+        <v>92807453</v>
       </c>
       <c r="F4" t="n">
-        <v>10018093002</v>
+        <v>10118873035</v>
       </c>
     </row>
     <row r="5">
@@ -548,22 +548,70 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Henning Berg</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>festningsgata 12</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>90806450</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8127995110</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Berit Andresen</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Festningsgata 2</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>90832301</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10018093002</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Lars Arne Holt</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Jeving veien 4</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E7" t="n">
         <v>90492508</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F7" t="n">
         <v>12108795110</v>
       </c>
     </row>
@@ -752,7 +800,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -786,9 +834,18 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -801,7 +858,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,33 +933,33 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Fjelltoppen barnehage</t>
+          <t>ABC Kindergarten</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2024-08-18</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>800000</t>
+          <t>2000000</t>
         </is>
       </c>
     </row>
@@ -911,25 +968,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
@@ -937,17 +986,58 @@
           <t>Fjelltoppen barnehage</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2024-08-18</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>on</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Fjelltoppen barnehage</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>2020-09-18</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="M4" t="n">
         <v>1500000</v>
       </c>
     </row>

</xml_diff>